<commit_message>
completed work except readme
</commit_message>
<xml_diff>
--- a/country_rank_table.xlsx
+++ b/country_rank_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geran\Projects\ais_fishing_signal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A923298-B2C4-48B6-9F91-FC254F316893}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6A539DA-B5A1-44EE-8045-CBBE4368795A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1395" yWindow="1260" windowWidth="23340" windowHeight="15345" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="75">
   <si>
     <t>flag</t>
   </si>
@@ -252,6 +252,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -315,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -323,11 +326,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.000"/>
+    </dxf>
     <dxf>
       <font>
         <b/>
@@ -385,15 +392,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{ADD03070-B460-42A1-ABD8-F5BE576B61D1}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0" headerRowDxfId="0" headerRowBorderDxfId="1" tableBorderDxfId="2">
-  <autoFilter ref="A1:C32" xr:uid="{ADD03070-B460-42A1-ABD8-F5BE576B61D1}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6906BBDC-3DF5-4417-8E67-611769831B35}" name="Table1" displayName="Table1" ref="A1:D32" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="2" tableBorderDxfId="3">
+  <autoFilter ref="A1:D32" xr:uid="{6906BBDC-3DF5-4417-8E67-611769831B35}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D32">
     <sortCondition ref="B1:B32"/>
   </sortState>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{4260B5B7-9960-496E-BAEF-B15C47F1C4A4}" name="SOVEREIGNT"/>
-    <tableColumn id="2" xr3:uid="{D2490048-C6E8-47A7-8DAA-0E9197603D0B}" name="rank"/>
-    <tableColumn id="3" xr3:uid="{C51B977E-401B-41F4-BCC5-9B3078361121}" name="spike_index"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{305255DD-0E3C-481A-9F25-8C68F408EB2D}" name="SOVEREIGNT"/>
+    <tableColumn id="2" xr3:uid="{BF5E4FB0-9768-439F-8413-C56FDCEA6527}" name="rank"/>
+    <tableColumn id="3" xr3:uid="{08BE3F11-9413-45A4-A766-185E4CF1CCDA}" name="spike_index" dataDxfId="0"/>
+    <tableColumn id="4" xr3:uid="{D8AD8C3B-FB4E-44DF-B885-6096BB9C6B15}" name="p_value"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -684,15 +692,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:O32"/>
+      <selection activeCell="J1" sqref="J1:M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -732,14 +740,8 @@
       <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -756,13 +758,13 @@
         <v>7.7138575289224001</v>
       </c>
       <c r="F2">
-        <v>3898</v>
+        <v>4248</v>
       </c>
       <c r="G2">
-        <v>1077.7693637253051</v>
+        <v>990.0349254769917</v>
       </c>
       <c r="H2">
-        <v>2.616729266200871</v>
+        <v>3.2907577204444021</v>
       </c>
       <c r="I2">
         <v>18835.861479530849</v>
@@ -771,7 +773,7 @@
         <v>0</v>
       </c>
       <c r="K2">
-        <v>10.330586795123271</v>
+        <v>11.0046152493668</v>
       </c>
       <c r="L2">
         <v>2</v>
@@ -779,14 +781,8 @@
       <c r="M2" t="s">
         <v>14</v>
       </c>
-      <c r="N2">
-        <v>2</v>
-      </c>
-      <c r="O2">
-        <v>10.330586795123271</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>15</v>
       </c>
@@ -803,13 +799,13 @@
         <v>2.520267525773848</v>
       </c>
       <c r="F3">
-        <v>1860</v>
+        <v>2327</v>
       </c>
       <c r="G3">
-        <v>851.34753895232734</v>
+        <v>787.96266142382865</v>
       </c>
       <c r="H3">
-        <v>1.184771688291864</v>
+        <v>1.9531856189672361</v>
       </c>
       <c r="I3">
         <v>4246.6964237837065</v>
@@ -818,22 +814,16 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>3.7050392140657129</v>
+        <v>4.4734531447410841</v>
       </c>
       <c r="L3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c r="N3">
-        <v>8</v>
-      </c>
-      <c r="O3">
-        <v>3.7050392140657129</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -850,13 +840,13 @@
         <v>6.7747760526641239</v>
       </c>
       <c r="F4">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="G4">
-        <v>283.63046691459778</v>
+        <v>258.78741940819651</v>
       </c>
       <c r="H4">
-        <v>2.1660914631938719</v>
+        <v>2.4738937544022139</v>
       </c>
       <c r="I4">
         <v>3583.7614108370112</v>
@@ -865,7 +855,7 @@
         <v>0</v>
       </c>
       <c r="K4">
-        <v>8.9408675158579953</v>
+        <v>9.2486698070663387</v>
       </c>
       <c r="L4">
         <v>3</v>
@@ -873,14 +863,8 @@
       <c r="M4" t="s">
         <v>18</v>
       </c>
-      <c r="N4">
-        <v>3</v>
-      </c>
-      <c r="O4">
-        <v>8.9408675158579953</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -897,13 +881,13 @@
         <v>-0.32992120300431138</v>
       </c>
       <c r="F5">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="G5">
-        <v>256.20647153319311</v>
+        <v>229.73639480108201</v>
       </c>
       <c r="H5">
-        <v>-0.30915094009610689</v>
+        <v>-0.20778769007154779</v>
       </c>
       <c r="I5">
         <v>835.72875548944069</v>
@@ -912,22 +896,16 @@
         <v>3.3255257727727731E-146</v>
       </c>
       <c r="K5">
-        <v>-0.63907214310041838</v>
+        <v>-0.53770889307585923</v>
       </c>
       <c r="L5">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="M5" t="s">
         <v>20</v>
       </c>
-      <c r="N5">
-        <v>27</v>
-      </c>
-      <c r="O5">
-        <v>-0.63907214310041838</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -944,13 +922,13 @@
         <v>7.9895387897027659</v>
       </c>
       <c r="F6">
-        <v>758</v>
+        <v>742</v>
       </c>
       <c r="G6">
-        <v>189.74293387508291</v>
+        <v>168.8630285089441</v>
       </c>
       <c r="H6">
-        <v>2.9948786735796382</v>
+        <v>3.3940938792335982</v>
       </c>
       <c r="I6">
         <v>3279.837153358586</v>
@@ -959,7 +937,7 @@
         <v>0</v>
       </c>
       <c r="K6">
-        <v>10.9844174632824</v>
+        <v>11.383632668936359</v>
       </c>
       <c r="L6">
         <v>1</v>
@@ -967,14 +945,8 @@
       <c r="M6" t="s">
         <v>22</v>
       </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-      <c r="O6">
-        <v>10.9844174632824</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -991,13 +963,13 @@
         <v>0.76841327162460971</v>
       </c>
       <c r="F7">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="G7">
-        <v>114.2043210960141</v>
+        <v>101.3248977547381</v>
       </c>
       <c r="H7">
-        <v>0.33970412442949111</v>
+        <v>0.59881730541815026</v>
       </c>
       <c r="I7">
         <v>150.90965498999341</v>
@@ -1006,7 +978,7 @@
         <v>2.323703169194095E-13</v>
       </c>
       <c r="K7">
-        <v>1.1081173960541011</v>
+        <v>1.36723057704276</v>
       </c>
       <c r="L7">
         <v>15</v>
@@ -1014,14 +986,8 @@
       <c r="M7" t="s">
         <v>24</v>
       </c>
-      <c r="N7">
-        <v>15</v>
-      </c>
-      <c r="O7">
-        <v>1.1081173960541011</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1038,13 +1004,13 @@
         <v>6.5308798933917958E-2</v>
       </c>
       <c r="F8">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="G8">
-        <v>67.649299371117095</v>
+        <v>64.158199399139235</v>
       </c>
       <c r="H8">
-        <v>3.4748336652937133E-2</v>
+        <v>0.1689854251272242</v>
       </c>
       <c r="I8">
         <v>149.4749244601407</v>
@@ -1053,22 +1019,16 @@
         <v>3.8914923443220499E-13</v>
       </c>
       <c r="K8">
-        <v>0.1000571355868551</v>
+        <v>0.2342942240611422</v>
       </c>
       <c r="L8">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M8" t="s">
         <v>26</v>
       </c>
-      <c r="N8">
-        <v>21</v>
-      </c>
-      <c r="O8">
-        <v>0.1000571355868551</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -1085,13 +1045,13 @@
         <v>2.2223449164324069</v>
       </c>
       <c r="F9">
-        <v>131</v>
+        <v>175</v>
       </c>
       <c r="G9">
-        <v>67.137493914999851</v>
+        <v>62.678680735332158</v>
       </c>
       <c r="H9">
-        <v>0.95121968904371024</v>
+        <v>1.792017922951463</v>
       </c>
       <c r="I9">
         <v>376.97973768513577</v>
@@ -1100,22 +1060,16 @@
         <v>5.4170400833752757E-54</v>
       </c>
       <c r="K9">
-        <v>3.1735646054761171</v>
+        <v>4.0143628393838702</v>
       </c>
       <c r="L9">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M9" t="s">
         <v>28</v>
       </c>
-      <c r="N9">
-        <v>9</v>
-      </c>
-      <c r="O9">
-        <v>3.1735646054761171</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1132,13 +1086,13 @@
         <v>0.73902024287645829</v>
       </c>
       <c r="F10">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G10">
-        <v>53.530878313616547</v>
+        <v>50.703838234919488</v>
       </c>
       <c r="H10">
-        <v>0.4197413230312721</v>
+        <v>0.53834507830773581</v>
       </c>
       <c r="I10">
         <v>113.4916512660334</v>
@@ -1147,22 +1101,16 @@
         <v>7.7276646201021589E-8</v>
       </c>
       <c r="K10">
-        <v>1.1587615659077299</v>
+        <v>1.277365321184194</v>
       </c>
       <c r="L10">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="M10" t="s">
         <v>30</v>
       </c>
-      <c r="N10">
-        <v>14</v>
-      </c>
-      <c r="O10">
-        <v>1.1587615659077299</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1179,13 +1127,13 @@
         <v>3.498377505176363</v>
       </c>
       <c r="F11">
-        <v>186</v>
+        <v>235</v>
       </c>
       <c r="G11">
-        <v>53.492568580128633</v>
+        <v>48.952332409156369</v>
       </c>
       <c r="H11">
-        <v>2.477118503318517</v>
+        <v>3.800588418051436</v>
       </c>
       <c r="I11">
         <v>760.09906162433799</v>
@@ -1194,22 +1142,16 @@
         <v>1.1515457424133669E-130</v>
       </c>
       <c r="K11">
-        <v>5.9754960084948792</v>
+        <v>7.298965923227799</v>
       </c>
       <c r="L11">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="M11" t="s">
         <v>32</v>
       </c>
-      <c r="N11">
-        <v>7</v>
-      </c>
-      <c r="O11">
-        <v>5.9754960084948792</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>33</v>
       </c>
@@ -1226,13 +1168,13 @@
         <v>-0.35658731016183748</v>
       </c>
       <c r="F12">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="G12">
-        <v>42.577909475459222</v>
+        <v>34.541998405226892</v>
       </c>
       <c r="H12">
-        <v>-0.15449113299586861</v>
+        <v>-0.36309417475188799</v>
       </c>
       <c r="I12">
         <v>132.94478908110131</v>
@@ -1241,7 +1183,7 @@
         <v>1.277847155386835E-10</v>
       </c>
       <c r="K12">
-        <v>-0.51107844315770612</v>
+        <v>-0.71968148491372563</v>
       </c>
       <c r="L12">
         <v>26</v>
@@ -1249,14 +1191,8 @@
       <c r="M12" t="s">
         <v>34</v>
       </c>
-      <c r="N12">
-        <v>26</v>
-      </c>
-      <c r="O12">
-        <v>-0.51107844315770612</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
@@ -1273,13 +1209,13 @@
         <v>0.84672384150218405</v>
       </c>
       <c r="F13">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="G13">
-        <v>48.903105979800962</v>
+        <v>44.174362706008942</v>
       </c>
       <c r="H13">
-        <v>0.49274772097608849</v>
+        <v>1.0373808355532319</v>
       </c>
       <c r="I13">
         <v>146.67494164914589</v>
@@ -1288,22 +1224,16 @@
         <v>1.058653362176696E-12</v>
       </c>
       <c r="K13">
-        <v>1.339471562478272</v>
+        <v>1.884104677055416</v>
       </c>
       <c r="L13">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="M13" t="s">
         <v>36</v>
       </c>
-      <c r="N13">
-        <v>13</v>
-      </c>
-      <c r="O13">
-        <v>1.339471562478272</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -1320,13 +1250,13 @@
         <v>1.646023481246796</v>
       </c>
       <c r="F14">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="G14">
-        <v>36.324199669988793</v>
+        <v>34.213739689674533</v>
       </c>
       <c r="H14">
-        <v>0.89956009015686877</v>
+        <v>0.54908526459605467</v>
       </c>
       <c r="I14">
         <v>77.765554885107989</v>
@@ -1335,22 +1265,16 @@
         <v>1.741953561015464E-3</v>
       </c>
       <c r="K14">
-        <v>2.545583571403665</v>
+        <v>2.19510874584285</v>
       </c>
       <c r="L14">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M14" t="s">
         <v>38</v>
       </c>
-      <c r="N14">
-        <v>11</v>
-      </c>
-      <c r="O14">
-        <v>2.545583571403665</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -1367,13 +1291,13 @@
         <v>1.040526244072945</v>
       </c>
       <c r="F15">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="G15">
-        <v>41.308791309207891</v>
+        <v>37.302354482625013</v>
       </c>
       <c r="H15">
-        <v>1.081881296314527</v>
+        <v>1.7076038872303509</v>
       </c>
       <c r="I15">
         <v>167.48747416638011</v>
@@ -1382,7 +1306,7 @@
         <v>5.2904697202137466E-16</v>
       </c>
       <c r="K15">
-        <v>2.122407540387472</v>
+        <v>2.748130131303296</v>
       </c>
       <c r="L15">
         <v>12</v>
@@ -1390,14 +1314,8 @@
       <c r="M15" t="s">
         <v>40</v>
       </c>
-      <c r="N15">
-        <v>12</v>
-      </c>
-      <c r="O15">
-        <v>2.122407540387472</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1414,13 +1332,13 @@
         <v>-0.66300822912842738</v>
       </c>
       <c r="F16">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="G16">
-        <v>27.173233692289521</v>
+        <v>21.62501101622998</v>
       </c>
       <c r="H16">
-        <v>-0.22718067942135239</v>
+        <v>-0.49132973889611942</v>
       </c>
       <c r="I16">
         <v>164.15167545891211</v>
@@ -1429,7 +1347,7 @@
         <v>1.8320697500891392E-15</v>
       </c>
       <c r="K16">
-        <v>-0.89018890854977983</v>
+        <v>-1.1543379680245469</v>
       </c>
       <c r="L16">
         <v>28</v>
@@ -1437,14 +1355,8 @@
       <c r="M16" t="s">
         <v>42</v>
       </c>
-      <c r="N16">
-        <v>28</v>
-      </c>
-      <c r="O16">
-        <v>-0.89018890854977983</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -1461,13 +1373,13 @@
         <v>-0.37469662353165722</v>
       </c>
       <c r="F17">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G17">
-        <v>33.815056620443762</v>
+        <v>29.290681187412211</v>
       </c>
       <c r="H17">
-        <v>-0.5564106200274298</v>
+        <v>-0.55617283473807355</v>
       </c>
       <c r="I17">
         <v>234.92604918410169</v>
@@ -1476,22 +1388,16 @@
         <v>1.5814421739509831E-27</v>
       </c>
       <c r="K17">
-        <v>-0.93110724355908703</v>
+        <v>-0.93086945826973078</v>
       </c>
       <c r="L17">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="M17" t="s">
         <v>44</v>
       </c>
-      <c r="N17">
-        <v>29</v>
-      </c>
-      <c r="O17">
-        <v>-0.93110724355908703</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>45</v>
       </c>
@@ -1508,13 +1414,13 @@
         <v>0.1650942870180992</v>
       </c>
       <c r="F18">
-        <v>35</v>
+        <v>13</v>
       </c>
       <c r="G18">
-        <v>26.175139327810879</v>
+        <v>20.95640879236301</v>
       </c>
       <c r="H18">
-        <v>0.33714665513977921</v>
+        <v>-0.37966470644829697</v>
       </c>
       <c r="I18">
         <v>81.615819261941681</v>
@@ -1523,22 +1429,16 @@
         <v>6.8497190366167038E-4</v>
       </c>
       <c r="K18">
-        <v>0.5022409421578784</v>
+        <v>-0.21457041943019781</v>
       </c>
       <c r="L18">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="M18" t="s">
         <v>46</v>
       </c>
-      <c r="N18">
-        <v>17</v>
-      </c>
-      <c r="O18">
-        <v>0.5022409421578784</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>47</v>
       </c>
@@ -1555,13 +1455,13 @@
         <v>-0.76840315693553563</v>
       </c>
       <c r="F19">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>26.302763219127581</v>
+        <v>21.243013789734601</v>
       </c>
       <c r="H19">
-        <v>0.48273394985508139</v>
+        <v>-0.90585140038055834</v>
       </c>
       <c r="I19">
         <v>102.76127915093311</v>
@@ -1570,22 +1470,16 @@
         <v>2.0740819479484338E-6</v>
       </c>
       <c r="K19">
-        <v>-0.28566920708045418</v>
+        <v>-1.6742545573160941</v>
       </c>
       <c r="L19">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="M19" t="s">
         <v>48</v>
       </c>
-      <c r="N19">
-        <v>24</v>
-      </c>
-      <c r="O19">
-        <v>-0.28566920708045418</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>49</v>
       </c>
@@ -1602,13 +1496,13 @@
         <v>-1</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G20">
-        <v>15.853128461524021</v>
+        <v>11.871082476055941</v>
       </c>
       <c r="H20">
-        <v>-0.93692096784385315</v>
+        <v>-1</v>
       </c>
       <c r="I20">
         <v>109.658644777226</v>
@@ -1617,7 +1511,7 @@
         <v>2.559596277738206E-7</v>
       </c>
       <c r="K20">
-        <v>-1.936920967843853</v>
+        <v>-2</v>
       </c>
       <c r="L20">
         <v>30</v>
@@ -1625,14 +1519,8 @@
       <c r="M20" t="s">
         <v>50</v>
       </c>
-      <c r="N20">
-        <v>30</v>
-      </c>
-      <c r="O20">
-        <v>-1.936920967843853</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -1649,13 +1537,13 @@
         <v>1.255770904104301E-2</v>
       </c>
       <c r="F21">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G21">
-        <v>17.791372461039639</v>
+        <v>16.92967044212573</v>
       </c>
       <c r="H21">
-        <v>0.23655440569166911</v>
+        <v>4.1542189562810928E-3</v>
       </c>
       <c r="I21">
         <v>107.5731058090968</v>
@@ -1664,7 +1552,7 @@
         <v>4.8612279711749045E-7</v>
       </c>
       <c r="K21">
-        <v>0.24911211473271211</v>
+        <v>1.67119279973241E-2</v>
       </c>
       <c r="L21">
         <v>20</v>
@@ -1672,14 +1560,8 @@
       <c r="M21" t="s">
         <v>52</v>
       </c>
-      <c r="N21">
-        <v>20</v>
-      </c>
-      <c r="O21">
-        <v>0.24911211473271211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -1696,13 +1578,13 @@
         <v>6.0918526060405744</v>
       </c>
       <c r="F22">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G22">
-        <v>22.939929723255819</v>
+        <v>20.494953429978889</v>
       </c>
       <c r="H22">
-        <v>1.920671545566131</v>
+        <v>2.3178899494610872</v>
       </c>
       <c r="I22">
         <v>241.68735747227819</v>
@@ -1711,7 +1593,7 @@
         <v>9.8433916989341214E-29</v>
       </c>
       <c r="K22">
-        <v>8.0125241516067049</v>
+        <v>8.4097425555016603</v>
       </c>
       <c r="L22">
         <v>4</v>
@@ -1719,14 +1601,8 @@
       <c r="M22" t="s">
         <v>54</v>
       </c>
-      <c r="N22">
-        <v>4</v>
-      </c>
-      <c r="O22">
-        <v>8.0125241516067049</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -1746,10 +1622,10 @@
         <v>49</v>
       </c>
       <c r="G23">
-        <v>20.450197847655399</v>
+        <v>18.016759715133279</v>
       </c>
       <c r="H23">
-        <v>1.396064838346678</v>
+        <v>1.7196899317496119</v>
       </c>
       <c r="I23">
         <v>146.6373755287695</v>
@@ -1758,22 +1634,16 @@
         <v>1.0729098675030251E-12</v>
       </c>
       <c r="K23">
-        <v>6.1479310949254851</v>
+        <v>6.4715561883284201</v>
       </c>
       <c r="L23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="M23" t="s">
         <v>56</v>
       </c>
-      <c r="N23">
-        <v>6</v>
-      </c>
-      <c r="O23">
-        <v>6.1479310949254851</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>57</v>
       </c>
@@ -1790,13 +1660,13 @@
         <v>0.57101890826349289</v>
       </c>
       <c r="F24">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="G24">
-        <v>19.25415589793235</v>
+        <v>16.448029200031218</v>
       </c>
       <c r="H24">
-        <v>0.24648414229248539</v>
+        <v>0.1551535912864222</v>
       </c>
       <c r="I24">
         <v>142.47499727062521</v>
@@ -1805,22 +1675,16 @@
         <v>4.6833687888860463E-12</v>
       </c>
       <c r="K24">
-        <v>0.81750305055597827</v>
+        <v>0.72617249954991503</v>
       </c>
       <c r="L24">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="M24" t="s">
         <v>58</v>
       </c>
-      <c r="N24">
-        <v>16</v>
-      </c>
-      <c r="O24">
-        <v>0.81750305055597827</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1837,13 +1701,13 @@
         <v>-0.170601721028248</v>
       </c>
       <c r="F25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G25">
-        <v>14.612229530830749</v>
+        <v>12.29670963101181</v>
       </c>
       <c r="H25">
-        <v>-0.24720591222641319</v>
+        <v>-0.18677432418340581</v>
       </c>
       <c r="I25">
         <v>90.98957898854151</v>
@@ -1852,22 +1716,16 @@
         <v>5.9539677885869508E-5</v>
       </c>
       <c r="K25">
-        <v>-0.41780763325466119</v>
+        <v>-0.35737604521165378</v>
       </c>
       <c r="L25">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="M25" t="s">
         <v>60</v>
       </c>
-      <c r="N25">
-        <v>25</v>
-      </c>
-      <c r="O25">
-        <v>-0.41780763325466119</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>61</v>
       </c>
@@ -1884,13 +1742,13 @@
         <v>-9.5100713241383819E-2</v>
       </c>
       <c r="F26">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="G26">
-        <v>13.40829606824189</v>
+        <v>11.174919770612529</v>
       </c>
       <c r="H26">
-        <v>0.11871038077150781</v>
+        <v>-0.55256949466886995</v>
       </c>
       <c r="I26">
         <v>75.378475054677693</v>
@@ -1899,22 +1757,16 @@
         <v>3.0369569587785322E-3</v>
       </c>
       <c r="K26">
-        <v>2.360966753012397E-2</v>
+        <v>-0.64767020791025376</v>
       </c>
       <c r="L26">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="M26" t="s">
         <v>62</v>
       </c>
-      <c r="N26">
-        <v>22</v>
-      </c>
-      <c r="O26">
-        <v>2.360966753012397E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>63</v>
       </c>
@@ -1934,7 +1786,7 @@
         <v>0</v>
       </c>
       <c r="G27">
-        <v>5.1087147369164123</v>
+        <v>3.6079767889719561</v>
       </c>
       <c r="H27">
         <v>-1</v>
@@ -1949,19 +1801,13 @@
         <v>-2</v>
       </c>
       <c r="L27">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M27" t="s">
         <v>64</v>
       </c>
-      <c r="N27">
-        <v>31</v>
-      </c>
-      <c r="O27">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -1978,13 +1824,13 @@
         <v>2.0740816877085951E-2</v>
       </c>
       <c r="F28">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G28">
-        <v>8.9618410597125546</v>
+        <v>7.1816548135261389</v>
       </c>
       <c r="H28">
-        <v>-0.21891049468974619</v>
+        <v>-0.30378163113843148</v>
       </c>
       <c r="I28">
         <v>68.227176513709097</v>
@@ -1993,22 +1839,16 @@
         <v>1.4304669833618571E-2</v>
       </c>
       <c r="K28">
-        <v>-0.19816967781266021</v>
+        <v>-0.28304081426134559</v>
       </c>
       <c r="L28">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M28" t="s">
         <v>66</v>
       </c>
-      <c r="N28">
-        <v>23</v>
-      </c>
-      <c r="O28">
-        <v>-0.19816967781266021</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>67</v>
       </c>
@@ -2025,13 +1865,13 @@
         <v>4.9366646719670557</v>
       </c>
       <c r="F29">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G29">
-        <v>10.65311671970985</v>
+        <v>9.5650609137328111</v>
       </c>
       <c r="H29">
-        <v>2.097685012588391</v>
+        <v>2.13641494503482</v>
       </c>
       <c r="I29">
         <v>108.02685540044089</v>
@@ -2040,22 +1880,16 @@
         <v>4.230682538093861E-7</v>
       </c>
       <c r="K29">
-        <v>7.0343496845554467</v>
+        <v>7.0730796170018753</v>
       </c>
       <c r="L29">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="M29" t="s">
         <v>68</v>
       </c>
-      <c r="N29">
-        <v>5</v>
-      </c>
-      <c r="O29">
-        <v>7.0343496845554467</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>69</v>
       </c>
@@ -2072,13 +1906,13 @@
         <v>-6.1416673507844438E-2</v>
       </c>
       <c r="F30">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G30">
-        <v>6.3993985253833774</v>
+        <v>6.048323940803062</v>
       </c>
       <c r="H30">
-        <v>0.40638217237155499</v>
+        <v>1.1493557764490261</v>
       </c>
       <c r="I30">
         <v>88.5089219001282</v>
@@ -2087,22 +1921,16 @@
         <v>1.1614927458808501E-4</v>
       </c>
       <c r="K30">
-        <v>0.34496549886371047</v>
+        <v>1.087939102941182</v>
       </c>
       <c r="L30">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="M30" t="s">
         <v>70</v>
       </c>
-      <c r="N30">
-        <v>19</v>
-      </c>
-      <c r="O30">
-        <v>0.34496549886371047</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>71</v>
       </c>
@@ -2119,13 +1947,13 @@
         <v>1.7103642575983129</v>
       </c>
       <c r="F31">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="G31">
-        <v>5.5493632572100857</v>
+        <v>5.0702279485122306</v>
       </c>
       <c r="H31">
-        <v>1.3426111064381261</v>
+        <v>3.7335149905917691</v>
       </c>
       <c r="I31">
         <v>140.62168435734841</v>
@@ -2134,22 +1962,16 @@
         <v>8.9762150076725366E-12</v>
       </c>
       <c r="K31">
-        <v>3.0529753640364392</v>
+        <v>5.4438792481900817</v>
       </c>
       <c r="L31">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="M31" t="s">
         <v>72</v>
       </c>
-      <c r="N31">
-        <v>10</v>
-      </c>
-      <c r="O31">
-        <v>3.0529753640364392</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>73</v>
       </c>
@@ -2166,13 +1988,13 @@
         <v>0.57884177043416951</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="G32">
-        <v>3.8112764303006559</v>
+        <v>3.471954337180525</v>
       </c>
       <c r="H32">
-        <v>-0.2128621329722489</v>
+        <v>3.0323110963979438</v>
       </c>
       <c r="I32">
         <v>100.21652437006171</v>
@@ -2181,19 +2003,13 @@
         <v>4.3903270483525919E-6</v>
       </c>
       <c r="K32">
-        <v>0.36597963746192058</v>
+        <v>3.6111528668321129</v>
       </c>
       <c r="L32">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="M32" t="s">
         <v>74</v>
-      </c>
-      <c r="N32">
-        <v>18</v>
-      </c>
-      <c r="O32">
-        <v>0.36597963746192058</v>
       </c>
     </row>
   </sheetData>
@@ -2202,20 +2018,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9C505FB-F07A-47BF-9896-BCC1A76808D6}">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DE1EDF-406F-4737-938C-A067BAE08668}">
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A18" sqref="A18:C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>12</v>
       </c>
@@ -2225,346 +2043,442 @@
       <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>10.9844174632824</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="3">
+        <v>11.383632668936359</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3">
-        <v>10.330586795123271</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="3">
+        <v>11.0046152493668</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>8.9408675158579953</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="3">
+        <v>9.2486698070663387</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>54</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>8.0125241516067049</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="3">
+        <v>8.4097425555016603</v>
+      </c>
+      <c r="D5">
+        <v>9.8433916989341214E-29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>32</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-      <c r="C6">
-        <v>7.0343496845554467</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="3">
+        <v>7.298965923227799</v>
+      </c>
+      <c r="D6">
+        <v>1.1515457424133669E-130</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-      <c r="C7">
-        <v>6.1479310949254851</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="3">
+        <v>7.0730796170018753</v>
+      </c>
+      <c r="D7">
+        <v>4.230682538093861E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>56</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-      <c r="C8">
-        <v>5.9754960084948792</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="3">
+        <v>6.4715561883284201</v>
+      </c>
+      <c r="D8">
+        <v>1.0729098675030251E-12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>3.7050392140657129</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="3">
+        <v>5.4438792481900817</v>
+      </c>
+      <c r="D9">
+        <v>8.9762150076725366E-12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-      <c r="C10">
-        <v>3.1735646054761171</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="3">
+        <v>4.4734531447410841</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>28</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-      <c r="C11">
-        <v>3.0529753640364392</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="3">
+        <v>4.0143628393838702</v>
+      </c>
+      <c r="D11">
+        <v>5.4170400833752757E-54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-      <c r="C12">
-        <v>2.545583571403665</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="3">
+        <v>3.6111528668321129</v>
+      </c>
+      <c r="D12">
+        <v>4.3903270483525919E-6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
-      <c r="C13">
-        <v>2.122407540387472</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C13" s="3">
+        <v>2.748130131303296</v>
+      </c>
+      <c r="D13">
+        <v>5.2904697202137466E-16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
-      <c r="C14">
-        <v>1.339471562478272</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C14" s="3">
+        <v>2.19510874584285</v>
+      </c>
+      <c r="D14">
+        <v>1.741953561015464E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
-      <c r="C15">
-        <v>1.1587615659077299</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C15" s="3">
+        <v>1.884104677055416</v>
+      </c>
+      <c r="D15">
+        <v>1.058653362176696E-12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>1.1081173960541011</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="3">
+        <v>1.36723057704276</v>
+      </c>
+      <c r="D16">
+        <v>2.323703169194095E-13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>58</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
-      <c r="C17">
-        <v>0.81750305055597827</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="3">
+        <v>1.277365321184194</v>
+      </c>
+      <c r="D17">
+        <v>7.7276646201021589E-8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>46</v>
+        <v>70</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
-      <c r="C18">
-        <v>0.5022409421578784</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="3">
+        <v>1.087939102941182</v>
+      </c>
+      <c r="D18">
+        <v>1.1614927458808501E-4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>74</v>
+        <v>58</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
-      <c r="C19">
-        <v>0.36597963746192058</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="3">
+        <v>0.72617249954991503</v>
+      </c>
+      <c r="D19">
+        <v>4.6833687888860463E-12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>26</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
-      <c r="C20">
-        <v>0.34496549886371047</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="3">
+        <v>0.2342942240611422</v>
+      </c>
+      <c r="D20">
+        <v>3.8914923443220499E-13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>52</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
-      <c r="C21">
-        <v>0.24911211473271211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="3">
+        <v>1.67119279973241E-2</v>
+      </c>
+      <c r="D21">
+        <v>4.8612279711749045E-7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
-      <c r="C22">
-        <v>0.1000571355868551</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="3">
+        <v>-0.21457041943019781</v>
+      </c>
+      <c r="D22">
+        <v>6.8497190366167038E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
-      <c r="C23">
-        <v>2.360966753012397E-2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="3">
+        <v>-0.28304081426134559</v>
+      </c>
+      <c r="D23">
+        <v>1.4304669833618571E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
-      <c r="C24">
-        <v>-0.19816967781266021</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="3">
+        <v>-0.35737604521165378</v>
+      </c>
+      <c r="D24">
+        <v>5.9539677885869508E-5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
-      <c r="C25">
-        <v>-0.28566920708045418</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="3">
+        <v>-0.53770889307585923</v>
+      </c>
+      <c r="D25">
+        <v>3.3255257727727731E-146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
-      <c r="C26">
-        <v>-0.41780763325466119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="3">
+        <v>-0.64767020791025376</v>
+      </c>
+      <c r="D26">
+        <v>3.0369569587785322E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>34</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
-      <c r="C27">
-        <v>-0.51107844315770612</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="3">
+        <v>-0.71968148491372563</v>
+      </c>
+      <c r="D27">
+        <v>1.277847155386835E-10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
-      <c r="C28">
-        <v>-0.63907214310041838</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="3">
+        <v>-0.93086945826973078</v>
+      </c>
+      <c r="D28">
+        <v>1.5814421739509831E-27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>42</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
-      <c r="C29">
-        <v>-0.89018890854977983</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="3">
+        <v>-1.1543379680245469</v>
+      </c>
+      <c r="D29">
+        <v>1.8320697500891392E-15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
-      <c r="C30">
-        <v>-0.93110724355908703</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="3">
+        <v>-1.6742545573160941</v>
+      </c>
+      <c r="D30">
+        <v>2.0740819479484338E-6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>50</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
-      <c r="C31">
-        <v>-1.936920967843853</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="3">
+        <v>-2</v>
+      </c>
+      <c r="D31">
+        <v>2.559596277738206E-7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>64</v>
       </c>
       <c r="B32">
-        <v>31</v>
-      </c>
-      <c r="C32">
+        <v>30</v>
+      </c>
+      <c r="C32" s="3">
         <v>-2</v>
+      </c>
+      <c r="D32">
+        <v>9.367299133291786E-26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>